<commit_message>
am corectat calculul roe
</commit_message>
<xml_diff>
--- a/MedLife Revizuit.xlsx
+++ b/MedLife Revizuit.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roxana.presura\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\MedLife\MedLife---finance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44313877-B609-4F1C-A635-53AF95ECAC94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCF7CE1B-F14C-4972-BF26-D23E25C1F20F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ActivePasive" sheetId="1" r:id="rId1"/>
@@ -563,7 +563,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -593,7 +593,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -605,12 +605,6 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="3" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -632,7 +626,7 @@
     <xf numFmtId="2" fontId="11" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="10" fillId="2" borderId="4" xfId="3" applyNumberFormat="1" applyAlignment="1">
@@ -931,52 +925,52 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.88671875" customWidth="1"/>
+    <col min="1" max="1" width="3.85546875" customWidth="1"/>
     <col min="2" max="2" width="30" style="11" customWidth="1"/>
-    <col min="3" max="3" width="24.6640625" style="11" customWidth="1"/>
-    <col min="4" max="4" width="39.88671875" style="11" customWidth="1"/>
-    <col min="5" max="5" width="34.5546875" style="11" customWidth="1"/>
-    <col min="6" max="6" width="35.6640625" style="11" customWidth="1"/>
-    <col min="7" max="7" width="32.88671875" style="11" customWidth="1"/>
-    <col min="8" max="8" width="36.88671875" style="11" customWidth="1"/>
-    <col min="9" max="9" width="17.88671875" style="11" customWidth="1"/>
-    <col min="10" max="10" width="26.6640625" customWidth="1"/>
-    <col min="11" max="11" width="20.88671875" customWidth="1"/>
-    <col min="12" max="12" width="28.5546875" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" style="11" customWidth="1"/>
+    <col min="4" max="4" width="39.85546875" style="11" customWidth="1"/>
+    <col min="5" max="5" width="34.5703125" style="11" customWidth="1"/>
+    <col min="6" max="6" width="35.7109375" style="11" customWidth="1"/>
+    <col min="7" max="7" width="32.85546875" style="11" customWidth="1"/>
+    <col min="8" max="8" width="36.85546875" style="11" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" style="11" customWidth="1"/>
+    <col min="10" max="10" width="26.7109375" customWidth="1"/>
+    <col min="11" max="11" width="20.85546875" customWidth="1"/>
+    <col min="12" max="12" width="28.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B1" s="14"/>
     </row>
-    <row r="2" spans="2:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="23" t="s">
+    <row r="2" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="23" t="s">
+      <c r="F2" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="23" t="s">
+      <c r="G2" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="H2" s="23" t="s">
+      <c r="H2" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="I2" s="23" t="s">
+      <c r="I2" s="21" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="3" spans="2:9" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:9" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="6" t="s">
         <v>6</v>
       </c>
@@ -996,7 +990,7 @@
       <c r="H3" s="15"/>
       <c r="I3" s="16"/>
     </row>
-    <row r="4" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="6" t="s">
         <v>7</v>
       </c>
@@ -1012,13 +1006,13 @@
       <c r="F4" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G4" s="17">
+      <c r="G4" s="16">
         <v>132562338</v>
       </c>
       <c r="H4" s="15"/>
       <c r="I4" s="16"/>
     </row>
-    <row r="5" spans="2:9" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="6" t="s">
         <v>8</v>
       </c>
@@ -1040,7 +1034,7 @@
       <c r="H5" s="15"/>
       <c r="I5" s="16"/>
     </row>
-    <row r="6" spans="2:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="6" t="s">
         <v>10</v>
       </c>
@@ -1062,7 +1056,7 @@
       <c r="H6" s="15"/>
       <c r="I6" s="16"/>
     </row>
-    <row r="7" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="6" t="s">
         <v>61</v>
       </c>
@@ -1078,40 +1072,40 @@
       <c r="F7" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="G7" s="17">
+      <c r="G7" s="16">
         <v>69593507</v>
       </c>
       <c r="H7" s="15"/>
       <c r="I7" s="16"/>
     </row>
-    <row r="8" spans="2:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="6" t="s">
         <v>62</v>
       </c>
       <c r="C8" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="D8" s="17">
+      <c r="D8" s="16">
         <v>112808224</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>77</v>
       </c>
       <c r="F8" s="13"/>
-      <c r="G8" s="17">
+      <c r="G8" s="16">
         <v>72018957</v>
       </c>
       <c r="H8" s="15"/>
       <c r="I8" s="16"/>
     </row>
-    <row r="9" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="6" t="s">
         <v>12</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D9" s="16">
         <v>17311896</v>
       </c>
       <c r="E9" s="6" t="s">
@@ -1125,7 +1119,7 @@
       <c r="H9" s="15"/>
       <c r="I9" s="16"/>
     </row>
-    <row r="10" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="6" t="s">
         <v>63</v>
       </c>
@@ -1138,7 +1132,7 @@
         <v>78</v>
       </c>
       <c r="F10" s="2"/>
-      <c r="G10" s="17">
+      <c r="G10" s="16">
         <v>571552330</v>
       </c>
       <c r="H10" s="15" t="s">
@@ -1148,21 +1142,21 @@
         <v>286025347</v>
       </c>
     </row>
-    <row r="11" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="D11" s="17">
+      <c r="D11" s="16">
         <v>1303969853</v>
       </c>
       <c r="E11" s="15" t="s">
         <v>79</v>
       </c>
       <c r="F11" s="2"/>
-      <c r="G11" s="17">
+      <c r="G11" s="16">
         <v>29076066</v>
       </c>
       <c r="H11" s="15" t="s">
@@ -1172,7 +1166,7 @@
         <v>69109052</v>
       </c>
     </row>
-    <row r="12" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="6" t="s">
         <v>16</v>
       </c>
@@ -1186,7 +1180,7 @@
         <v>80</v>
       </c>
       <c r="F12" s="13"/>
-      <c r="G12" s="17">
+      <c r="G12" s="16">
         <v>108288263</v>
       </c>
       <c r="H12" s="15" t="s">
@@ -1196,14 +1190,14 @@
         <v>1135073779</v>
       </c>
     </row>
-    <row r="13" spans="2:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="15" t="s">
         <v>64</v>
       </c>
       <c r="C13" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="D13" s="17">
+      <c r="D13" s="16">
         <v>492034979</v>
       </c>
       <c r="E13" s="6" t="s">
@@ -1220,34 +1214,34 @@
         <v>45236597</v>
       </c>
     </row>
-    <row r="14" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="15" t="s">
         <v>66</v>
       </c>
       <c r="C14" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="D14" s="17">
+      <c r="D14" s="16">
         <v>54138411</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>82</v>
       </c>
       <c r="F14" s="13"/>
-      <c r="G14" s="17">
+      <c r="G14" s="16">
         <v>4322327</v>
       </c>
       <c r="H14" s="15"/>
       <c r="I14" s="16"/>
     </row>
-    <row r="15" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="15" t="s">
         <v>67</v>
       </c>
       <c r="C15" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="D15" s="17">
+      <c r="D15" s="16">
         <v>0</v>
       </c>
       <c r="E15" s="6" t="s">
@@ -1260,14 +1254,14 @@
       <c r="H15" s="15"/>
       <c r="I15" s="16"/>
     </row>
-    <row r="16" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="15" t="s">
         <v>66</v>
       </c>
       <c r="C16" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="D16" s="17">
+      <c r="D16" s="16">
         <v>386290334</v>
       </c>
       <c r="E16" s="6" t="s">
@@ -1280,34 +1274,33 @@
       <c r="H16" s="15"/>
       <c r="I16" s="16"/>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B17" s="19" t="s">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="19"/>
-      <c r="D17" s="20">
+      <c r="C17" s="17"/>
+      <c r="D17" s="18">
         <f>D10 +D3</f>
         <v>3016313845</v>
       </c>
-      <c r="E17" s="19" t="s">
+      <c r="E17" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="F17" s="21"/>
-      <c r="G17" s="20">
+      <c r="F17" s="19"/>
+      <c r="G17" s="18">
         <f xml:space="preserve"> G3 +G9 +I17</f>
         <v>3016313845</v>
       </c>
-      <c r="H17" s="21" t="s">
+      <c r="H17" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="I17" s="27">
+      <c r="I17" s="25">
         <f xml:space="preserve"> SUM(I10:I13)</f>
         <v>1535444775</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="14"/>
-      <c r="C18" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1319,39 +1312,39 @@
   <dimension ref="B2:E26"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.77734375" style="5" customWidth="1"/>
-    <col min="2" max="2" width="21.5546875" style="22" customWidth="1"/>
-    <col min="3" max="3" width="22.109375" style="22" customWidth="1"/>
-    <col min="4" max="4" width="23.5546875" style="22" customWidth="1"/>
-    <col min="5" max="5" width="28.109375" style="22" customWidth="1"/>
-    <col min="6" max="16384" width="9.109375" style="5"/>
+    <col min="1" max="1" width="3.7109375" style="5" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" style="20" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" style="20" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" style="20" customWidth="1"/>
+    <col min="5" max="5" width="28.140625" style="20" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="24"/>
-      <c r="D2" s="25" t="s">
+    <row r="2" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="22"/>
+      <c r="D2" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="23" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="2:5" ht="45.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="24" t="s">
+    <row r="3" spans="2:5" ht="45.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="22" t="s">
         <v>21</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
     </row>
-    <row r="4" spans="2:5" ht="29.4" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="26">
+    <row r="4" spans="2:5" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="24">
         <v>1</v>
       </c>
       <c r="C4" s="13" t="s">
@@ -1360,13 +1353,13 @@
       <c r="D4" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="26">
+      <c r="E4" s="24">
         <f>658905448 / 976224339</f>
         <v>0.67495289932532609</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B5" s="26">
+    <row r="5" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B5" s="24">
         <v>2</v>
       </c>
       <c r="C5" s="13" t="s">
@@ -1375,13 +1368,13 @@
       <c r="D5" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="26">
+      <c r="E5" s="24">
         <f>(658905448 - 148798218) / 976224339</f>
         <v>0.52253074382731612</v>
       </c>
     </row>
-    <row r="6" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B6" s="26">
+    <row r="6" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B6" s="24">
         <v>3</v>
       </c>
       <c r="C6" s="13" t="s">
@@ -1390,27 +1383,27 @@
       <c r="D6" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="26">
+      <c r="E6" s="24">
         <f>112808224 / 976224339</f>
         <v>0.11555563561911972</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
     </row>
-    <row r="8" spans="2:5" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="24" t="s">
+    <row r="8" spans="2:5" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="22" t="s">
         <v>30</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
     </row>
-    <row r="9" spans="2:5" ht="29.4" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="26">
+    <row r="9" spans="2:5" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="24">
         <v>1</v>
       </c>
       <c r="C9" s="13" t="s">
@@ -1419,13 +1412,13 @@
       <c r="D9" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="26">
+      <c r="E9" s="24">
         <f>2511669114 / 3016313845</f>
         <v>0.83269488623124366</v>
       </c>
     </row>
-    <row r="10" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B10" s="26">
+    <row r="10" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B10" s="24">
         <v>2</v>
       </c>
       <c r="C10" s="13" t="s">
@@ -1434,13 +1427,13 @@
       <c r="D10" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="26">
+      <c r="E10" s="24">
         <f>2511669114 / 504644731</f>
         <v>4.9771036131158972</v>
       </c>
     </row>
-    <row r="11" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B11" s="26">
+    <row r="11" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B11" s="24">
         <v>3</v>
       </c>
       <c r="C11" s="13" t="s">
@@ -1449,13 +1442,13 @@
       <c r="D11" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="26">
+      <c r="E11" s="24">
         <f>3016313845 / 504644731</f>
         <v>5.9771036131158972</v>
       </c>
     </row>
-    <row r="12" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B12" s="26">
+    <row r="12" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B12" s="24">
         <v>4</v>
       </c>
       <c r="C12" s="13" t="s">
@@ -1464,13 +1457,13 @@
       <c r="D12" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="E12" s="26">
+      <c r="E12" s="24">
         <f>140408371 / 102630990</f>
         <v>1.3680894143182287</v>
       </c>
     </row>
-    <row r="13" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B13" s="26">
+    <row r="13" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B13" s="24">
         <v>5</v>
       </c>
       <c r="C13" s="13" t="s">
@@ -1479,27 +1472,27 @@
       <c r="D13" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="E13" s="26">
+      <c r="E13" s="24">
         <f>401476411 / 102630990</f>
         <v>3.9118438884785189</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
     </row>
-    <row r="15" spans="2:5" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="24" t="s">
+    <row r="15" spans="2:5" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="22" t="s">
         <v>40</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
     </row>
-    <row r="16" spans="2:5" ht="29.4" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="26">
+    <row r="16" spans="2:5" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="24">
         <v>1</v>
       </c>
       <c r="C16" s="13" t="s">
@@ -1508,13 +1501,13 @@
       <c r="D16" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="E16" s="26">
+      <c r="E16" s="24">
         <f>725787350 / 148798218</f>
         <v>4.8776615725330794</v>
       </c>
     </row>
-    <row r="17" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B17" s="26">
+    <row r="17" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B17" s="24">
         <v>2</v>
       </c>
       <c r="C17" s="13" t="s">
@@ -1523,13 +1516,13 @@
       <c r="D17" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="E17" s="26">
+      <c r="E17" s="24">
         <f>365 / E16</f>
         <v>74.830939902713936</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B18" s="26">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="24">
         <v>3</v>
       </c>
       <c r="C18" s="13" t="s">
@@ -1538,13 +1531,13 @@
       <c r="D18" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="E18" s="26">
+      <c r="E18" s="24">
         <f>2715574711 / 324106860</f>
         <v>8.3786400294026482</v>
       </c>
     </row>
-    <row r="19" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B19" s="26">
+    <row r="19" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B19" s="24">
         <v>4</v>
       </c>
       <c r="C19" s="13" t="s">
@@ -1553,13 +1546,13 @@
       <c r="D19" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="E19" s="26">
+      <c r="E19" s="24">
         <f>365 / 8.38</f>
         <v>43.556085918854414</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B20" s="26">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="24">
         <v>5</v>
       </c>
       <c r="C20" s="13" t="s">
@@ -1568,13 +1561,13 @@
       <c r="D20" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="E20" s="26">
+      <c r="E20" s="24">
         <f>2715574711 / 3016313845</f>
         <v>0.90029580824338917</v>
       </c>
     </row>
-    <row r="21" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B21" s="26">
+    <row r="21" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B21" s="24">
         <v>6</v>
       </c>
       <c r="C21" s="13" t="s">
@@ -1583,27 +1576,27 @@
       <c r="D21" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="E21" s="26">
+      <c r="E21" s="24">
         <f>3016313845 / 2715574711</f>
         <v>1.1107460357403511</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
     </row>
-    <row r="23" spans="2:5" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="24" t="s">
+    <row r="23" spans="2:5" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="22" t="s">
         <v>53</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
     </row>
-    <row r="24" spans="2:5" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="26">
+    <row r="24" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="24">
         <v>1</v>
       </c>
       <c r="C24" s="13" t="s">
@@ -1612,13 +1605,13 @@
       <c r="D24" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="E24" s="26">
+      <c r="E24" s="24">
         <f>16752427 / 2715574711</f>
         <v>6.1690171631591691E-3</v>
       </c>
     </row>
-    <row r="25" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B25" s="26">
+    <row r="25" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B25" s="24">
         <v>2</v>
       </c>
       <c r="C25" s="13" t="s">
@@ -1627,13 +1620,13 @@
       <c r="D25" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="E25" s="26">
+      <c r="E25" s="24">
         <f>16752427 / 3016313845</f>
         <v>5.5539402929737237E-3</v>
       </c>
     </row>
-    <row r="26" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B26" s="26">
+    <row r="26" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B26" s="24">
         <v>3</v>
       </c>
       <c r="C26" s="13" t="s">
@@ -1642,7 +1635,7 @@
       <c r="D26" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="E26" s="26">
+      <c r="E26" s="24">
         <f>25035987 / 432625774</f>
         <v>5.7869846191826751E-2</v>
       </c>
@@ -1658,38 +1651,38 @@
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.77734375" customWidth="1"/>
-    <col min="2" max="2" width="36.88671875" customWidth="1"/>
-    <col min="3" max="3" width="29.88671875" customWidth="1"/>
-    <col min="4" max="4" width="42.33203125" customWidth="1"/>
-    <col min="5" max="5" width="9.109375" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="2" max="2" width="36.85546875" customWidth="1"/>
+    <col min="3" max="3" width="29.85546875" customWidth="1"/>
+    <col min="4" max="4" width="42.28515625" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="28" t="s">
+    <row r="2" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="26" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="2:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>89</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="D3" s="29">
+      <c r="D3" s="27">
         <v>2715574711</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>91</v>
       </c>
@@ -1700,7 +1693,7 @@
         <v>8850263</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>95</v>
       </c>
@@ -1712,18 +1705,18 @@
         <v>2724424974</v>
       </c>
     </row>
-    <row r="6" spans="2:4" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:4" ht="180" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>92</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="D6" s="29">
+      <c r="D6" s="27">
         <v>2584016603</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>94</v>
       </c>
@@ -1735,7 +1728,7 @@
         <v>140408371</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>14</v>
       </c>
@@ -1747,7 +1740,7 @@
         <v>401476411</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>98</v>
       </c>
@@ -1758,7 +1751,7 @@
         <v>102630990</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>99</v>
       </c>
@@ -1769,7 +1762,7 @@
         <v>2175920</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>100</v>
       </c>
@@ -1780,7 +1773,7 @@
         <v>462070</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>101</v>
       </c>
@@ -1791,7 +1784,7 @@
         <v>1346241</v>
       </c>
     </row>
-    <row r="13" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>102</v>
       </c>
@@ -1803,7 +1796,7 @@
         <v>-101339241</v>
       </c>
     </row>
-    <row r="14" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>103</v>
       </c>
@@ -1815,7 +1808,7 @@
         <v>39069130</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>104</v>
       </c>
@@ -1826,7 +1819,7 @@
         <v>22316703</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>18</v>
       </c>
@@ -1838,7 +1831,7 @@
         <v>16752427</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>105</v>
       </c>
@@ -1849,7 +1842,7 @@
         <v>25035987</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>106</v>
       </c>

</xml_diff>